<commit_message>
actualizando todas las tareas semana ultima de marzo
</commit_message>
<xml_diff>
--- a/CUADRANTE LIMPIEZA CASA.xlsx
+++ b/CUADRANTE LIMPIEZA CASA.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0014371\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0014371\Documents\MADRID VIAJE VIEWNEXT\Cuadrante casa\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16962" windowHeight="7147"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16962" windowHeight="7147" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla" sheetId="5" r:id="rId1"/>
@@ -17,11 +17,11 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Datos!$A$1:$E$19</definedName>
-    <definedName name="_xlcn.WorksheetConnection_Hoja1AE" hidden="1">Datos!$A:$E</definedName>
+    <definedName name="_xlcn.WorksheetConnection_Hoja1AE1" hidden="1">Datos!$A:$E</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="153" r:id="rId3"/>
+    <pivotCache cacheId="3" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -53,7 +53,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Rango" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Hoja1AE"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Hoja1AE1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="27">
   <si>
     <t>Baño P1</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Recuento de Hecho</t>
+  </si>
+  <si>
+    <t>Total 21</t>
   </si>
 </sst>
 </file>
@@ -298,244 +301,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="125">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
+  <dxfs count="50">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -708,7 +474,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="INSA" refreshedDate="43180.682549189813" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="INSA" refreshedDate="43194.549385763887" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="5">
     <cacheField name="[Rango].[Persona].[Persona]" caption="Persona" numFmtId="0" hierarchy="3" level="1">
@@ -722,13 +488,13 @@
       </sharedItems>
     </cacheField>
     <cacheField name="[Rango].[Zonas].[Zonas]" caption="Zonas" numFmtId="0" hierarchy="2" level="1">
-      <sharedItems containsNonDate="0" count="6">
+      <sharedItems count="6">
         <s v="Baño P0"/>
-        <s v="Baño P1" u="1"/>
-        <s v="Baño P-1" u="1"/>
-        <s v="Cocina" u="1"/>
-        <s v="Salon" u="1"/>
-        <s v="Suelo global" u="1"/>
+        <s v="Baño P1"/>
+        <s v="Baño P-1"/>
+        <s v="Cocina"/>
+        <s v="Salon"/>
+        <s v="Suelo global"/>
       </sharedItems>
     </cacheField>
     <cacheField name="[Rango].[Mes].[Mes]" caption="Mes" numFmtId="0" hierarchy="1" level="1">
@@ -740,7 +506,7 @@
     <cacheField name="[Rango].[Día].[Día]" caption="Día" numFmtId="0" level="1">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="5" maxValue="21" count="3">
         <n v="15"/>
-        <n v="21" u="1"/>
+        <n v="21"/>
         <n v="5" u="1"/>
       </sharedItems>
       <extLst>
@@ -814,8 +580,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="153" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" colHeaderCaption="">
-  <location ref="A1:D11" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" colHeaderCaption="">
+  <location ref="A1:K11" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
       <items count="7">
@@ -887,10 +653,32 @@
     <field x="3"/>
     <field x="1"/>
   </colFields>
-  <colItems count="3">
+  <colItems count="10">
     <i>
       <x/>
       <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="5"/>
+    </i>
+    <i t="default" r="1">
+      <x v="2"/>
     </i>
     <i t="default">
       <x/>
@@ -903,7 +691,7 @@
     <dataField name="Recuento de Hecho" fld="4" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="25">
-    <format dxfId="124">
+    <format dxfId="49">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -915,7 +703,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="123">
+    <format dxfId="48">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -927,58 +715,58 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="122">
+    <format dxfId="47">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="121">
+    <format dxfId="46">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="120">
+    <format dxfId="45">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="119">
+    <format dxfId="44">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="118">
+    <format dxfId="43">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="117">
+    <format dxfId="42">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="2"/>
     </format>
-    <format dxfId="116">
+    <format dxfId="41">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="115">
+    <format dxfId="40">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="114">
+    <format dxfId="39">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="113">
+    <format dxfId="38">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="112">
+    <format dxfId="37">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="111">
+    <format dxfId="36">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0" defaultSubtotal="1"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="110">
+    <format dxfId="35">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="109">
+    <format dxfId="34">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -991,7 +779,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="108">
+    <format dxfId="33">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -1004,7 +792,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="107">
+    <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -1016,7 +804,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="106">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -1028,7 +816,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="105">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -1040,7 +828,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="104">
+    <format dxfId="29">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -1052,7 +840,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="103">
+    <format dxfId="28">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="1" count="0"/>
@@ -1065,7 +853,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="102">
+    <format dxfId="27">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="1" count="0"/>
@@ -1078,7 +866,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="101">
+    <format dxfId="26">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="1" count="0"/>
@@ -1091,7 +879,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="100">
+    <format dxfId="25">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="1" count="0"/>
@@ -1400,23 +1188,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="18.4609375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3828125" customWidth="1"/>
-    <col min="4" max="4" width="11.3046875" customWidth="1"/>
-    <col min="5" max="5" width="10.3828125" customWidth="1"/>
-    <col min="6" max="6" width="11.3046875" customWidth="1"/>
-    <col min="7" max="7" width="10.4609375" customWidth="1"/>
-    <col min="8" max="10" width="7.3046875" customWidth="1"/>
-    <col min="11" max="11" width="10.3828125" customWidth="1"/>
+    <col min="3" max="4" width="7.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.15234375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.4609375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.3046875" customWidth="1"/>
+    <col min="10" max="10" width="10.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.3046875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.3046875" customWidth="1"/>
     <col min="13" max="13" width="5.15234375" customWidth="1"/>
     <col min="14" max="14" width="10.4609375" customWidth="1"/>
@@ -1439,7 +1228,7 @@
     <col min="33" max="33" width="11.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
         <v>25</v>
       </c>
@@ -1448,50 +1237,105 @@
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="13"/>
       <c r="B2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="K2" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="13"/>
       <c r="B3" s="14">
         <v>15</v>
       </c>
-      <c r="C3" s="13"/>
+      <c r="C3" s="13">
+        <v>21</v>
+      </c>
       <c r="D3" s="13"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>2</v>
+      </c>
+      <c r="K5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
@@ -1501,67 +1345,122 @@
       <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2</v>
+      </c>
+      <c r="K6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
+      <c r="C7" s="1"/>
       <c r="D7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>2</v>
+      </c>
+      <c r="K7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>2</v>
+      </c>
+      <c r="K8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2</v>
+      </c>
+      <c r="K9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1">
+        <v>2</v>
+      </c>
+      <c r="K10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" s="13" t="s">
         <v>20</v>
       </c>
@@ -1569,10 +1468,31 @@
         <v>6</v>
       </c>
       <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
         <v>6</v>
       </c>
-      <c r="D11" s="1">
-        <v>6</v>
+      <c r="J11" s="1">
+        <v>12</v>
+      </c>
+      <c r="K11" s="1">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1584,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1725,7 +1645,9 @@
       <c r="D8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="11"/>
+      <c r="E8" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="5">
@@ -1740,7 +1662,9 @@
       <c r="D9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="11"/>
+      <c r="E9" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="5">
@@ -1755,7 +1679,9 @@
       <c r="D10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="11"/>
+      <c r="E10" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="5">
@@ -1770,7 +1696,9 @@
       <c r="D11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="11"/>
+      <c r="E11" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="5">
@@ -1785,7 +1713,9 @@
       <c r="D12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="11"/>
+      <c r="E12" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="15.05" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="8">
@@ -1800,7 +1730,9 @@
       <c r="D13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="11"/>
+      <c r="E13" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2">
@@ -1893,46 +1825,94 @@
       <c r="E19" s="11"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
+      <c r="A20" s="2">
+        <v>12</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="E20" s="11"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
+      <c r="A21" s="5">
+        <v>12</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="E21" s="11"/>
       <c r="I21" s="15"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
+      <c r="A22" s="5">
+        <v>12</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="E22" s="11"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="7"/>
+      <c r="A23" s="5">
+        <v>12</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="E23" s="11"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="7"/>
+      <c r="A24" s="5">
+        <v>12</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="E24" s="11"/>
     </row>
     <row r="25" spans="1:9" ht="15.05" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="8"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="10"/>
+      <c r="A25" s="8">
+        <v>12</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="E25" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fran actualiza cuadrante 5 abril
</commit_message>
<xml_diff>
--- a/CUADRANTE LIMPIEZA CASA.xlsx
+++ b/CUADRANTE LIMPIEZA CASA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16962" windowHeight="7147" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16962" windowHeight="7147"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Datos!$A$1:$E$19</definedName>
-    <definedName name="_xlcn.WorksheetConnection_Hoja1AE1" hidden="1">Datos!$A:$E</definedName>
+    <definedName name="_xlcn.WorksheetConnection_Hoja1AE" hidden="1">Datos!$A:$E</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
@@ -53,7 +53,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Rango" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Hoja1AE1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Hoja1AE"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="29">
   <si>
     <t>Baño P1</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>Total 21</t>
+  </si>
+  <si>
+    <t>Total Abril</t>
+  </si>
+  <si>
+    <t>Total 5</t>
   </si>
 </sst>
 </file>
@@ -301,86 +307,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
+  <dxfs count="25">
     <dxf>
       <alignment horizontal="center" readingOrder="0"/>
     </dxf>
@@ -474,7 +401,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="INSA" refreshedDate="43194.549385763887" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="INSA" refreshedDate="43195.386109490741" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="5">
     <cacheField name="[Rango].[Persona].[Persona]" caption="Persona" numFmtId="0" hierarchy="3" level="1">
@@ -489,9 +416,9 @@
     </cacheField>
     <cacheField name="[Rango].[Zonas].[Zonas]" caption="Zonas" numFmtId="0" hierarchy="2" level="1">
       <sharedItems count="6">
-        <s v="Baño P0"/>
         <s v="Baño P1"/>
         <s v="Baño P-1"/>
+        <s v="Baño P0"/>
         <s v="Cocina"/>
         <s v="Salon"/>
         <s v="Suelo global"/>
@@ -499,22 +426,22 @@
     </cacheField>
     <cacheField name="[Rango].[Mes].[Mes]" caption="Mes" numFmtId="0" hierarchy="1" level="1">
       <sharedItems count="2">
+        <s v="Abril"/>
         <s v="Marzo"/>
-        <s v="Abril" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="[Rango].[Día].[Día]" caption="Día" numFmtId="0" level="1">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="5" maxValue="21" count="3">
+        <n v="5"/>
         <n v="15"/>
         <n v="21"/>
-        <n v="5" u="1"/>
       </sharedItems>
       <extLst>
         <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{4F2E5C28-24EA-4eb8-9CBF-B6C8F9C3D259}">
           <x15:cachedUniqueNames>
-            <x15:cachedUniqueName index="0" name="[Rango].[Día].&amp;[15]"/>
-            <x15:cachedUniqueName index="1" name="[Rango].[Día].&amp;[21]"/>
-            <x15:cachedUniqueName index="2" name="[Rango].[Día].&amp;[5]"/>
+            <x15:cachedUniqueName index="0" name="[Rango].[Día].&amp;[5]"/>
+            <x15:cachedUniqueName index="1" name="[Rango].[Día].&amp;[15]"/>
+            <x15:cachedUniqueName index="2" name="[Rango].[Día].&amp;[21]"/>
           </x15:cachedUniqueNames>
         </ext>
       </extLst>
@@ -581,7 +508,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" colHeaderCaption="">
-  <location ref="A1:K11" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
+  <location ref="A1:O11" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
       <items count="7">
@@ -596,9 +523,9 @@
     </pivotField>
     <pivotField axis="axisCol" allDrilled="1" showAll="0" sortType="ascending" defaultAttributeDrillState="1">
       <items count="7">
+        <item s="1" x="2"/>
         <item s="1" x="0"/>
         <item s="1" x="1"/>
-        <item s="1" x="2"/>
         <item s="1" x="3"/>
         <item s="1" x="4"/>
         <item s="1" x="5"/>
@@ -607,16 +534,16 @@
     </pivotField>
     <pivotField axis="axisCol" allDrilled="1" showAll="0" sortType="ascending" defaultAttributeDrillState="1">
       <items count="3">
+        <item x="1"/>
         <item x="0"/>
-        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisCol" allDrilled="1" showAll="0" sortType="ascending" defaultAttributeDrillState="1">
       <items count="4">
+        <item x="0"/>
+        <item x="1" e="0"/>
         <item x="2"/>
-        <item x="0" e="0"/>
-        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -653,7 +580,7 @@
     <field x="3"/>
     <field x="1"/>
   </colFields>
-  <colItems count="10">
+  <colItems count="14">
     <i>
       <x/>
       <x v="1"/>
@@ -682,6 +609,20 @@
     </i>
     <i t="default">
       <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i t="default">
+      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
@@ -691,7 +632,7 @@
     <dataField name="Recuento de Hecho" fld="4" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="25">
-    <format dxfId="49">
+    <format dxfId="24">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -703,7 +644,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="23">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -715,58 +656,58 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="47">
+    <format dxfId="22">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="46">
+    <format dxfId="21">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="45">
+    <format dxfId="20">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="44">
+    <format dxfId="19">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="18">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="17">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="2"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="16">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="40">
+    <format dxfId="15">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="39">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="37">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="36">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0" defaultSubtotal="1"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="35">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -779,7 +720,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -792,7 +733,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -804,7 +745,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -816,7 +757,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="5">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -828,7 +769,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -840,7 +781,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="1" count="0"/>
@@ -853,7 +794,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="1" count="0"/>
@@ -866,7 +807,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="1" count="0"/>
@@ -879,7 +820,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="1" count="0"/>
@@ -1188,10 +1129,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1205,11 +1146,11 @@
     <col min="8" max="8" width="10.4609375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.3046875" customWidth="1"/>
     <col min="10" max="10" width="10.3828125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.3046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.3046875" customWidth="1"/>
-    <col min="13" max="13" width="5.15234375" customWidth="1"/>
-    <col min="14" max="14" width="10.4609375" customWidth="1"/>
-    <col min="15" max="15" width="7.3046875" customWidth="1"/>
+    <col min="11" max="11" width="7.3046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.3046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.07421875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.3046875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.3828125" customWidth="1"/>
     <col min="17" max="18" width="7.3046875" customWidth="1"/>
     <col min="19" max="19" width="7.921875" customWidth="1"/>
@@ -1228,7 +1169,7 @@
     <col min="33" max="33" width="11.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
         <v>25</v>
       </c>
@@ -1244,8 +1185,12 @@
       <c r="I1" s="13"/>
       <c r="J1" s="13"/>
       <c r="K1" s="13"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="13"/>
       <c r="B2" s="13" t="s">
         <v>14</v>
@@ -1261,10 +1206,18 @@
         <v>22</v>
       </c>
       <c r="K2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="13"/>
       <c r="B3" s="14">
         <v>15</v>
@@ -1281,9 +1234,17 @@
         <v>26</v>
       </c>
       <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K3" s="13">
+        <v>5</v>
+      </c>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" s="12" t="s">
         <v>18</v>
       </c>
@@ -1308,9 +1269,17 @@
       </c>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" s="13" t="s">
         <v>8</v>
       </c>
@@ -1332,10 +1301,20 @@
         <v>2</v>
       </c>
       <c r="K5" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1">
+        <v>1</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
@@ -1356,11 +1335,21 @@
       <c r="J6" s="1">
         <v>2</v>
       </c>
-      <c r="K6" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K6" s="1"/>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
+      <c r="N6" s="1">
+        <v>1</v>
+      </c>
+      <c r="O6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" s="13" t="s">
         <v>6</v>
       </c>
@@ -1381,11 +1370,15 @@
       <c r="J7" s="1">
         <v>2</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" s="13" t="s">
         <v>10</v>
       </c>
@@ -1406,11 +1399,15 @@
       <c r="J8" s="1">
         <v>2</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" s="13" t="s">
         <v>7</v>
       </c>
@@ -1431,11 +1428,15 @@
       <c r="J9" s="1">
         <v>2</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" s="13" t="s">
         <v>19</v>
       </c>
@@ -1456,11 +1457,15 @@
       <c r="J10" s="1">
         <v>2</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" s="13" t="s">
         <v>20</v>
       </c>
@@ -1492,7 +1497,19 @@
         <v>12</v>
       </c>
       <c r="K11" s="1">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1">
+        <v>2</v>
+      </c>
+      <c r="N11" s="1">
+        <v>2</v>
+      </c>
+      <c r="O11" s="1">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1504,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1747,7 +1764,9 @@
       <c r="D14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="11"/>
+      <c r="E14" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="5">
@@ -1777,7 +1796,9 @@
       <c r="D16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="11"/>
+      <c r="E16" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="5">

</xml_diff>

<commit_message>
tareas compeltadas 5 abril
</commit_message>
<xml_diff>
--- a/CUADRANTE LIMPIEZA CASA.xlsx
+++ b/CUADRANTE LIMPIEZA CASA.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0014367\Desktop\Excel-tareas-casa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0014371\Documents\MADRID VIAJE VIEWNEXT\Cuadrante casa\Excel-tareas-casa\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16968" windowHeight="7152" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16971" windowHeight="7156"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla" sheetId="5" r:id="rId1"/>
@@ -17,11 +17,11 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Datos!$A$1:$E$19</definedName>
-    <definedName name="_xlcn.WorksheetConnection_Hoja1AE1" hidden="1">Datos!$A:$E</definedName>
+    <definedName name="_xlcn.WorksheetConnection_Hoja1AE" hidden="1">Datos!$A:$E</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId3"/>
+    <pivotCache cacheId="3" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -53,7 +53,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Rango" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Hoja1AE1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Hoja1AE"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="30">
   <si>
     <t>Baño P1</t>
   </si>
@@ -310,165 +310,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="100">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
+  <dxfs count="50">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -641,7 +483,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="INSA" refreshedDate="43195.737539120368" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="INSA" refreshedDate="43199.458510069446" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="5">
     <cacheField name="[Rango].[Persona].[Persona]" caption="Persona" numFmtId="0" hierarchy="3" level="1">
@@ -656,9 +498,9 @@
     </cacheField>
     <cacheField name="[Rango].[Zonas].[Zonas]" caption="Zonas" numFmtId="0" hierarchy="2" level="1">
       <sharedItems count="6">
+        <s v="Baño P0"/>
         <s v="Baño P1"/>
         <s v="Baño P-1"/>
-        <s v="Baño P0"/>
         <s v="Cocina"/>
         <s v="Salon"/>
         <s v="Suelo global"/>
@@ -747,8 +589,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" colHeaderCaption="">
-  <location ref="A1:U11" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" colHeaderCaption="">
+  <location ref="A1:Y11" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
       <items count="7">
@@ -763,9 +605,9 @@
     </pivotField>
     <pivotField axis="axisCol" allDrilled="1" showAll="0" sortType="ascending" defaultAttributeDrillState="1">
       <items count="7">
-        <item s="1" x="2"/>
         <item s="1" x="0"/>
         <item s="1" x="1"/>
+        <item s="1" x="2"/>
         <item s="1" x="3"/>
         <item s="1" x="4"/>
         <item s="1" x="5"/>
@@ -820,7 +662,7 @@
     <field x="3"/>
     <field x="1"/>
   </colFields>
-  <colItems count="20">
+  <colItems count="24">
     <i>
       <x/>
       <x v="1"/>
@@ -872,10 +714,22 @@
     <i>
       <x v="1"/>
       <x/>
+      <x/>
+    </i>
+    <i r="2">
       <x v="1"/>
     </i>
     <i r="2">
       <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="5"/>
     </i>
     <i t="default" r="1">
       <x/>
@@ -891,7 +745,7 @@
     <dataField name="Recuento de Hecho" fld="4" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="25">
-    <format dxfId="99">
+    <format dxfId="49">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -903,7 +757,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="98">
+    <format dxfId="48">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -915,58 +769,58 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="97">
+    <format dxfId="47">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="96">
+    <format dxfId="46">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="95">
+    <format dxfId="45">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="94">
+    <format dxfId="44">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="93">
+    <format dxfId="43">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="92">
+    <format dxfId="42">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="2"/>
     </format>
-    <format dxfId="91">
+    <format dxfId="41">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="90">
+    <format dxfId="40">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="89">
+    <format dxfId="39">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="38">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="87">
+    <format dxfId="37">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="36">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0" defaultSubtotal="1"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="85">
+    <format dxfId="35">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="84">
+    <format dxfId="34">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -979,7 +833,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="33">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -992,7 +846,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -1004,7 +858,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="81">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -1016,7 +870,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -1028,7 +882,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="29">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -1040,7 +894,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="28">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="1" count="0"/>
@@ -1053,7 +907,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="27">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="1" count="0"/>
@@ -1066,7 +920,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="26">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="1" count="0"/>
@@ -1079,7 +933,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="25">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="1" count="0"/>
@@ -1388,48 +1242,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U11"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.44140625" customWidth="1"/>
-    <col min="23" max="23" width="6.33203125" customWidth="1"/>
-    <col min="24" max="24" width="9.109375" customWidth="1"/>
-    <col min="25" max="26" width="7.33203125" customWidth="1"/>
-    <col min="27" max="27" width="7.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.4609375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.15234375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.4609375" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="7.3046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.15234375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.4609375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.3046875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.3828125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="7.3046875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.921875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.15234375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.4609375" customWidth="1"/>
+    <col min="23" max="23" width="6.3046875" customWidth="1"/>
+    <col min="24" max="24" width="9.07421875" customWidth="1"/>
+    <col min="25" max="25" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.3046875" customWidth="1"/>
+    <col min="27" max="27" width="7.84375" customWidth="1"/>
     <col min="28" max="28" width="6" customWidth="1"/>
-    <col min="29" max="29" width="5.109375" customWidth="1"/>
-    <col min="30" max="30" width="10.44140625" customWidth="1"/>
-    <col min="31" max="31" width="6.33203125" customWidth="1"/>
-    <col min="32" max="32" width="9.88671875" customWidth="1"/>
-    <col min="33" max="33" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.07421875" customWidth="1"/>
+    <col min="30" max="30" width="10.4609375" customWidth="1"/>
+    <col min="31" max="31" width="6.3046875" customWidth="1"/>
+    <col min="32" max="32" width="9.84375" customWidth="1"/>
+    <col min="33" max="33" width="11.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
         <v>25</v>
       </c>
@@ -1455,8 +1308,12 @@
       <c r="S1" s="13"/>
       <c r="T1" s="13"/>
       <c r="U1" s="13"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A2" s="13"/>
       <c r="B2" s="13" t="s">
         <v>14</v>
@@ -1482,14 +1339,18 @@
       </c>
       <c r="R2" s="13"/>
       <c r="S2" s="13"/>
-      <c r="T2" s="13" t="s">
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="U2" s="13" t="s">
+      <c r="Y2" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A3" s="13"/>
       <c r="B3" s="14">
         <v>15</v>
@@ -1518,13 +1379,17 @@
         <v>5</v>
       </c>
       <c r="R3" s="13"/>
-      <c r="S3" s="13" t="s">
-        <v>28</v>
-      </c>
+      <c r="S3" s="13"/>
       <c r="T3" s="13"/>
       <c r="U3" s="13"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V3" s="13"/>
+      <c r="W3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A4" s="12" t="s">
         <v>18</v>
       </c>
@@ -1568,16 +1433,28 @@
       <c r="O4" s="13"/>
       <c r="P4" s="13"/>
       <c r="Q4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="R4" s="13" t="s">
+      <c r="S4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="U4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="V4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="W4" s="13"/>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="13"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A5" s="13" t="s">
         <v>8</v>
       </c>
@@ -1606,21 +1483,25 @@
       <c r="P5" s="1">
         <v>2</v>
       </c>
-      <c r="Q5" s="1">
-        <v>1</v>
-      </c>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1">
-        <v>1</v>
-      </c>
-      <c r="T5" s="1">
-        <v>1</v>
-      </c>
-      <c r="U5" s="1">
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1">
+        <v>1</v>
+      </c>
+      <c r="X5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
@@ -1650,20 +1531,24 @@
         <v>2</v>
       </c>
       <c r="Q6" s="1"/>
-      <c r="R6" s="1">
-        <v>1</v>
-      </c>
+      <c r="R6" s="1"/>
       <c r="S6" s="1">
         <v>1</v>
       </c>
-      <c r="T6" s="1">
-        <v>1</v>
-      </c>
-      <c r="U6" s="1">
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1">
+        <v>1</v>
+      </c>
+      <c r="X6" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A7" s="13" t="s">
         <v>6</v>
       </c>
@@ -1692,15 +1577,25 @@
       <c r="P7" s="1">
         <v>2</v>
       </c>
-      <c r="Q7" s="1"/>
+      <c r="Q7" s="1">
+        <v>1</v>
+      </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
-      <c r="U7" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1">
+        <v>1</v>
+      </c>
+      <c r="X7" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A8" s="13" t="s">
         <v>10</v>
       </c>
@@ -1734,10 +1629,20 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1">
+        <v>1</v>
+      </c>
+      <c r="X8" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A9" s="13" t="s">
         <v>7</v>
       </c>
@@ -1769,12 +1674,22 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T9" s="1">
+        <v>1</v>
+      </c>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1">
+        <v>1</v>
+      </c>
+      <c r="X9" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A10" s="13" t="s">
         <v>19</v>
       </c>
@@ -1807,11 +1722,21 @@
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
-      <c r="U10" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U10" s="1"/>
+      <c r="V10" s="1">
+        <v>1</v>
+      </c>
+      <c r="W10" s="1">
+        <v>1</v>
+      </c>
+      <c r="X10" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A11" s="13" t="s">
         <v>20</v>
       </c>
@@ -1867,13 +1792,25 @@
         <v>1</v>
       </c>
       <c r="S11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U11" s="1">
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="V11" s="1">
+        <v>1</v>
+      </c>
+      <c r="W11" s="1">
+        <v>6</v>
+      </c>
+      <c r="X11" s="1">
+        <v>6</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1885,16 +1822,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.05" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1911,7 +1848,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="2">
         <v>15</v>
       </c>
@@ -1928,7 +1865,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="5">
         <v>15</v>
       </c>
@@ -1945,7 +1882,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="5">
         <v>15</v>
       </c>
@@ -1962,7 +1899,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="5">
         <v>15</v>
       </c>
@@ -1979,7 +1916,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="5">
         <v>15</v>
       </c>
@@ -1996,7 +1933,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="15.05" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="8">
         <v>15</v>
       </c>
@@ -2013,7 +1950,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="2">
         <v>21</v>
       </c>
@@ -2030,7 +1967,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="5">
         <v>21</v>
       </c>
@@ -2047,7 +1984,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="5">
         <v>21</v>
       </c>
@@ -2064,7 +2001,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="5">
         <v>21</v>
       </c>
@@ -2081,7 +2018,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="5">
         <v>21</v>
       </c>
@@ -2098,7 +2035,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="15.05" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="8">
         <v>21</v>
       </c>
@@ -2115,7 +2052,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2">
         <v>5</v>
       </c>
@@ -2132,7 +2069,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="5">
         <v>5</v>
       </c>
@@ -2145,9 +2082,11 @@
       <c r="D15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="11"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E15" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="5">
         <v>5</v>
       </c>
@@ -2164,7 +2103,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="5">
         <v>5</v>
       </c>
@@ -2181,7 +2120,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="5">
         <v>5</v>
       </c>
@@ -2194,9 +2133,11 @@
       <c r="D18" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E18" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.05" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="8">
         <v>5</v>
       </c>
@@ -2209,9 +2150,11 @@
       <c r="D19" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E19" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="2">
         <v>12</v>
       </c>
@@ -2226,7 +2169,7 @@
       </c>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="5">
         <v>12</v>
       </c>
@@ -2242,7 +2185,7 @@
       <c r="E21" s="11"/>
       <c r="I21" s="15"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="5">
         <v>12</v>
       </c>
@@ -2257,7 +2200,7 @@
       </c>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="5">
         <v>12</v>
       </c>
@@ -2272,7 +2215,7 @@
       </c>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="5">
         <v>12</v>
       </c>
@@ -2287,7 +2230,7 @@
       </c>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="15.05" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="8">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Dani ha limpiado baño P0 12 abril
</commit_message>
<xml_diff>
--- a/CUADRANTE LIMPIEZA CASA.xlsx
+++ b/CUADRANTE LIMPIEZA CASA.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0014371\Documents\MADRID VIAJE VIEWNEXT\Cuadrante casa\Excel-tareas-casa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0014372\Documents\CUADRANTE CASA\Excel-tareas-casa\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16971" windowHeight="7156"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16965" windowHeight="7155" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Datos!$A$1:$E$19</definedName>
-    <definedName name="_xlcn.WorksheetConnection_Hoja1AE" hidden="1">Datos!$A:$E</definedName>
+    <definedName name="_xlcn.WorksheetConnection_Hoja1AE1" hidden="1">Datos!$A:$E</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
@@ -53,7 +53,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Rango" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Hoja1AE"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Hoja1AE1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="31">
   <si>
     <t>Baño P1</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>Total 15</t>
+  </si>
+  <si>
+    <t>Total 12</t>
   </si>
 </sst>
 </file>
@@ -483,7 +486,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="INSA" refreshedDate="43199.458510069446" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="INSA" refreshedDate="43202.645456597224" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="5">
     <cacheField name="[Rango].[Persona].[Persona]" caption="Persona" numFmtId="0" hierarchy="3" level="1">
@@ -513,8 +516,9 @@
       </sharedItems>
     </cacheField>
     <cacheField name="[Rango].[Día].[Día]" caption="Día" numFmtId="0" level="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="5" maxValue="21" count="3">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="5" maxValue="21" count="4">
         <n v="5"/>
+        <n v="12"/>
         <n v="15"/>
         <n v="21"/>
       </sharedItems>
@@ -522,8 +526,9 @@
         <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{4F2E5C28-24EA-4eb8-9CBF-B6C8F9C3D259}">
           <x15:cachedUniqueNames>
             <x15:cachedUniqueName index="0" name="[Rango].[Día].&amp;[5]"/>
-            <x15:cachedUniqueName index="1" name="[Rango].[Día].&amp;[15]"/>
-            <x15:cachedUniqueName index="2" name="[Rango].[Día].&amp;[21]"/>
+            <x15:cachedUniqueName index="1" name="[Rango].[Día].&amp;[12]"/>
+            <x15:cachedUniqueName index="2" name="[Rango].[Día].&amp;[15]"/>
+            <x15:cachedUniqueName index="3" name="[Rango].[Día].&amp;[21]"/>
           </x15:cachedUniqueNames>
         </ext>
       </extLst>
@@ -590,7 +595,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" colHeaderCaption="">
-  <location ref="A1:Y11" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
+  <location ref="A1:AA11" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
       <items count="7">
@@ -622,10 +627,11 @@
       </items>
     </pivotField>
     <pivotField axis="axisCol" allDrilled="1" showAll="0" sortType="ascending" defaultAttributeDrillState="1">
-      <items count="4">
+      <items count="5">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
+        <item x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -662,10 +668,10 @@
     <field x="3"/>
     <field x="1"/>
   </colFields>
-  <colItems count="24">
+  <colItems count="26">
     <i>
       <x/>
-      <x v="1"/>
+      <x v="2"/>
       <x/>
     </i>
     <i r="2">
@@ -684,10 +690,10 @@
       <x v="5"/>
     </i>
     <i t="default" r="1">
-      <x v="1"/>
+      <x v="2"/>
     </i>
     <i r="1">
-      <x v="2"/>
+      <x v="3"/>
       <x/>
     </i>
     <i r="2">
@@ -706,7 +712,7 @@
       <x v="5"/>
     </i>
     <i t="default" r="1">
-      <x v="2"/>
+      <x v="3"/>
     </i>
     <i t="default">
       <x/>
@@ -733,6 +739,13 @@
     </i>
     <i t="default" r="1">
       <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i t="default" r="1">
+      <x v="1"/>
     </i>
     <i t="default">
       <x v="1"/>
@@ -752,7 +765,7 @@
             <x v="0"/>
           </reference>
           <reference field="3" count="1">
-            <x v="1"/>
+            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
@@ -764,7 +777,7 @@
             <x v="0"/>
           </reference>
           <reference field="3" count="1">
-            <x v="1"/>
+            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
@@ -827,8 +840,8 @@
             <x v="0"/>
           </reference>
           <reference field="3" count="2">
-            <x v="1"/>
             <x v="2"/>
+            <x v="3"/>
           </reference>
         </references>
       </pivotArea>
@@ -840,8 +853,8 @@
             <x v="0"/>
           </reference>
           <reference field="3" count="2" defaultSubtotal="1">
-            <x v="1"/>
             <x v="2"/>
+            <x v="3"/>
           </reference>
         </references>
       </pivotArea>
@@ -902,7 +915,7 @@
             <x v="0"/>
           </reference>
           <reference field="3" count="1" selected="0">
-            <x v="1"/>
+            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
@@ -915,7 +928,7 @@
             <x v="0"/>
           </reference>
           <reference field="3" count="1" selected="0">
-            <x v="2"/>
+            <x v="3"/>
           </reference>
         </references>
       </pivotArea>
@@ -1242,47 +1255,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y11"/>
+  <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.4609375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.15234375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.4609375" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="7.3046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.921875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.15234375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.4609375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.3046875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.3828125" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="7.3046875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.921875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.15234375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.4609375" customWidth="1"/>
-    <col min="23" max="23" width="6.3046875" customWidth="1"/>
-    <col min="24" max="24" width="9.07421875" customWidth="1"/>
-    <col min="25" max="25" width="11.3046875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.3046875" customWidth="1"/>
-    <col min="27" max="27" width="7.84375" customWidth="1"/>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="6" customWidth="1"/>
-    <col min="29" max="29" width="5.07421875" customWidth="1"/>
-    <col min="30" max="30" width="10.4609375" customWidth="1"/>
-    <col min="31" max="31" width="6.3046875" customWidth="1"/>
-    <col min="32" max="32" width="9.84375" customWidth="1"/>
-    <col min="33" max="33" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.140625" customWidth="1"/>
+    <col min="30" max="30" width="10.42578125" customWidth="1"/>
+    <col min="31" max="31" width="6.28515625" customWidth="1"/>
+    <col min="32" max="32" width="9.85546875" customWidth="1"/>
+    <col min="33" max="33" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>25</v>
       </c>
@@ -1312,8 +1326,10 @@
       <c r="W1" s="13"/>
       <c r="X1" s="13"/>
       <c r="Y1" s="13"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="13" t="s">
         <v>14</v>
@@ -1343,14 +1359,16 @@
       <c r="U2" s="13"/>
       <c r="V2" s="13"/>
       <c r="W2" s="13"/>
-      <c r="X2" s="13" t="s">
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="Y2" s="13" t="s">
+      <c r="AA2" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="14">
         <v>15</v>
@@ -1386,10 +1404,16 @@
       <c r="W3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="13"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="X3" s="13">
+        <v>12</v>
+      </c>
+      <c r="Y3" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="13"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>18</v>
       </c>
@@ -1451,10 +1475,14 @@
         <v>13</v>
       </c>
       <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
+      <c r="X4" s="13" t="s">
+        <v>1</v>
+      </c>
       <c r="Y4" s="13"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="Z4" s="13"/>
+      <c r="AA4" s="13"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>8</v>
       </c>
@@ -1498,10 +1526,16 @@
         <v>1</v>
       </c>
       <c r="Y5" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
@@ -1541,14 +1575,16 @@
       <c r="W6" s="1">
         <v>1</v>
       </c>
-      <c r="X6" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="1">
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>6</v>
       </c>
@@ -1588,14 +1624,16 @@
       <c r="W7" s="1">
         <v>1</v>
       </c>
-      <c r="X7" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="1">
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>10</v>
       </c>
@@ -1635,14 +1673,16 @@
       <c r="W8" s="1">
         <v>1</v>
       </c>
-      <c r="X8" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="1">
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>7</v>
       </c>
@@ -1682,14 +1722,16 @@
       <c r="W9" s="1">
         <v>1</v>
       </c>
-      <c r="X9" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y9" s="1">
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>19</v>
       </c>
@@ -1729,14 +1771,16 @@
       <c r="W10" s="1">
         <v>1</v>
       </c>
-      <c r="X10" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="1">
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>20</v>
       </c>
@@ -1807,10 +1851,16 @@
         <v>6</v>
       </c>
       <c r="X11" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="Y11" s="1">
-        <v>18</v>
+        <v>1</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>7</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1822,16 +1872,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="17.69140625" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.05" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1848,7 +1898,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>15</v>
       </c>
@@ -1865,7 +1915,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>15</v>
       </c>
@@ -1882,7 +1932,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>15</v>
       </c>
@@ -1899,7 +1949,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>15</v>
       </c>
@@ -1916,7 +1966,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>15</v>
       </c>
@@ -1933,7 +1983,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.05" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>15</v>
       </c>
@@ -1950,7 +2000,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>21</v>
       </c>
@@ -1967,7 +2017,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>21</v>
       </c>
@@ -1984,7 +2034,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>21</v>
       </c>
@@ -2001,7 +2051,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>21</v>
       </c>
@@ -2018,7 +2068,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>21</v>
       </c>
@@ -2035,7 +2085,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.05" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>21</v>
       </c>
@@ -2052,7 +2102,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>5</v>
       </c>
@@ -2069,7 +2119,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>5</v>
       </c>
@@ -2086,7 +2136,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>5</v>
       </c>
@@ -2103,7 +2153,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>5</v>
       </c>
@@ -2120,7 +2170,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>5</v>
       </c>
@@ -2137,7 +2187,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.05" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>5</v>
       </c>
@@ -2154,7 +2204,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>12</v>
       </c>
@@ -2169,7 +2219,7 @@
       </c>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>12</v>
       </c>
@@ -2182,10 +2232,12 @@
       <c r="D21" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="11"/>
+      <c r="E21" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="I21" s="15"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>12</v>
       </c>
@@ -2200,7 +2252,7 @@
       </c>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>12</v>
       </c>
@@ -2215,7 +2267,7 @@
       </c>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>12</v>
       </c>
@@ -2230,7 +2282,7 @@
       </c>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:9" ht="15.05" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
añadiendo tareas 19 abril
</commit_message>
<xml_diff>
--- a/CUADRANTE LIMPIEZA CASA.xlsx
+++ b/CUADRANTE LIMPIEZA CASA.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0014372\Documents\CUADRANTE CASA\Excel-tareas-casa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0014371\Documents\MADRID VIAJE VIEWNEXT\Cuadrante casa\Excel-tareas-casa\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16965" windowHeight="7155" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16962" windowHeight="7156"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla" sheetId="5" r:id="rId1"/>
@@ -17,11 +17,11 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Datos!$A$1:$E$19</definedName>
-    <definedName name="_xlcn.WorksheetConnection_Hoja1AE1" hidden="1">Datos!$A:$E</definedName>
+    <definedName name="_xlcn.WorksheetConnection_Hoja1AE" hidden="1">Datos!$A:$E</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId3"/>
+    <pivotCache cacheId="5" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -53,7 +53,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Rango" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Hoja1AE1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Hoja1AE"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="31">
   <si>
     <t>Baño P1</t>
   </si>
@@ -313,86 +313,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
+  <dxfs count="25">
     <dxf>
       <alignment horizontal="center" readingOrder="0"/>
     </dxf>
@@ -486,7 +407,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="INSA" refreshedDate="43202.645456597224" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="INSA" refreshedDate="43209.532398379626" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="5">
     <cacheField name="[Rango].[Persona].[Persona]" caption="Persona" numFmtId="0" hierarchy="3" level="1">
@@ -594,8 +515,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" colHeaderCaption="">
-  <location ref="A1:AA11" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" colHeaderCaption="">
+  <location ref="A1:AF11" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
       <items count="7">
@@ -668,7 +589,7 @@
     <field x="3"/>
     <field x="1"/>
   </colFields>
-  <colItems count="26">
+  <colItems count="31">
     <i>
       <x/>
       <x v="2"/>
@@ -743,6 +664,21 @@
     <i r="1">
       <x v="1"/>
       <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="5"/>
     </i>
     <i t="default" r="1">
       <x v="1"/>
@@ -758,7 +694,7 @@
     <dataField name="Recuento de Hecho" fld="4" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="25">
-    <format dxfId="49">
+    <format dxfId="24">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -770,7 +706,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="23">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -782,58 +718,58 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="47">
+    <format dxfId="22">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="46">
+    <format dxfId="21">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="45">
+    <format dxfId="20">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="44">
+    <format dxfId="19">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="18">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="17">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="2"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="16">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="40">
+    <format dxfId="15">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="39">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="37">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="36">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0" defaultSubtotal="1"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="35">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -846,7 +782,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -859,7 +795,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -871,7 +807,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -883,7 +819,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="5">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -895,7 +831,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -907,7 +843,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="1" count="0"/>
@@ -920,7 +856,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="1" count="0"/>
@@ -933,7 +869,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="1" count="0"/>
@@ -946,7 +882,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="1" count="0"/>
@@ -1255,48 +1191,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA11"/>
+  <dimension ref="A1:AF11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6" customWidth="1"/>
-    <col min="29" max="29" width="5.140625" customWidth="1"/>
-    <col min="30" max="30" width="10.42578125" customWidth="1"/>
-    <col min="31" max="31" width="6.28515625" customWidth="1"/>
-    <col min="32" max="32" width="9.85546875" customWidth="1"/>
-    <col min="33" max="33" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.4609375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.15234375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.4609375" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="7.3046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.15234375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.4609375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.3046875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.3828125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="7.3046875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.921875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.15234375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.4609375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.3046875" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="7.3046875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.921875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.15234375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.4609375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.3046875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.07421875" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="11.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
         <v>25</v>
       </c>
@@ -1328,8 +1261,13 @@
       <c r="Y1" s="13"/>
       <c r="Z1" s="13"/>
       <c r="AA1" s="13"/>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13"/>
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="13"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A2" s="13"/>
       <c r="B2" s="13" t="s">
         <v>14</v>
@@ -1361,14 +1299,19 @@
       <c r="W2" s="13"/>
       <c r="X2" s="13"/>
       <c r="Y2" s="13"/>
-      <c r="Z2" s="13" t="s">
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="13"/>
+      <c r="AC2" s="13"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="13" t="s">
+      <c r="AF2" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A3" s="13"/>
       <c r="B3" s="14">
         <v>15</v>
@@ -1407,13 +1350,18 @@
       <c r="X3" s="13">
         <v>12</v>
       </c>
-      <c r="Y3" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="Y3" s="13"/>
       <c r="Z3" s="13"/>
       <c r="AA3" s="13"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB3" s="13"/>
+      <c r="AC3" s="13"/>
+      <c r="AD3" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE3" s="13"/>
+      <c r="AF3" s="13"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A4" s="12" t="s">
         <v>18</v>
       </c>
@@ -1478,11 +1426,26 @@
       <c r="X4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="Y4" s="13"/>
-      <c r="Z4" s="13"/>
-      <c r="AA4" s="13"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Y4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD4" s="13"/>
+      <c r="AE4" s="13"/>
+      <c r="AF4" s="13"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A5" s="13" t="s">
         <v>8</v>
       </c>
@@ -1525,17 +1488,22 @@
       <c r="X5" s="1">
         <v>1</v>
       </c>
-      <c r="Y5" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="1">
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="1">
         <v>2</v>
       </c>
-      <c r="AA5" s="1">
+      <c r="AF5" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
@@ -1577,14 +1545,23 @@
       </c>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
-      <c r="Z6" s="1">
-        <v>1</v>
-      </c>
+      <c r="Z6" s="1"/>
       <c r="AA6" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>2</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A7" s="13" t="s">
         <v>6</v>
       </c>
@@ -1629,11 +1606,20 @@
       <c r="Z7" s="1">
         <v>1</v>
       </c>
-      <c r="AA7" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>2</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A8" s="13" t="s">
         <v>10</v>
       </c>
@@ -1675,14 +1661,23 @@
       </c>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
-      <c r="Z8" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA8" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="1">
+        <v>2</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A9" s="13" t="s">
         <v>7</v>
       </c>
@@ -1723,15 +1718,24 @@
         <v>1</v>
       </c>
       <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA9" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Y9" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="1">
+        <v>2</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A10" s="13" t="s">
         <v>19</v>
       </c>
@@ -1773,14 +1777,23 @@
       </c>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
-      <c r="Z10" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA10" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE10" s="1">
+        <v>2</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.4">
       <c r="A11" s="13" t="s">
         <v>20</v>
       </c>
@@ -1857,10 +1870,25 @@
         <v>1</v>
       </c>
       <c r="Z11" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="AA11" s="1">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>6</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>12</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1870,18 +1898,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.05" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1898,7 +1926,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="2">
         <v>15</v>
       </c>
@@ -1915,7 +1943,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="5">
         <v>15</v>
       </c>
@@ -1932,7 +1960,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="5">
         <v>15</v>
       </c>
@@ -1949,7 +1977,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="5">
         <v>15</v>
       </c>
@@ -1966,7 +1994,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="5">
         <v>15</v>
       </c>
@@ -1983,7 +2011,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15.05" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="8">
         <v>15</v>
       </c>
@@ -2000,7 +2028,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="2">
         <v>21</v>
       </c>
@@ -2017,7 +2045,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="5">
         <v>21</v>
       </c>
@@ -2034,7 +2062,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="5">
         <v>21</v>
       </c>
@@ -2051,7 +2079,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="5">
         <v>21</v>
       </c>
@@ -2068,7 +2096,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="5">
         <v>21</v>
       </c>
@@ -2085,7 +2113,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="15.05" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="8">
         <v>21</v>
       </c>
@@ -2102,7 +2130,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2">
         <v>5</v>
       </c>
@@ -2119,7 +2147,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="5">
         <v>5</v>
       </c>
@@ -2136,7 +2164,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="5">
         <v>5</v>
       </c>
@@ -2153,7 +2181,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="5">
         <v>5</v>
       </c>
@@ -2170,7 +2198,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="5">
         <v>5</v>
       </c>
@@ -2187,7 +2215,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15.05" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="8">
         <v>5</v>
       </c>
@@ -2204,7 +2232,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="2">
         <v>12</v>
       </c>
@@ -2217,9 +2245,11 @@
       <c r="D20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E20" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="5">
         <v>12</v>
       </c>
@@ -2237,7 +2267,7 @@
       </c>
       <c r="I21" s="15"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="5">
         <v>12</v>
       </c>
@@ -2250,9 +2280,11 @@
       <c r="D22" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="11"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E22" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="5">
         <v>12</v>
       </c>
@@ -2265,9 +2297,11 @@
       <c r="D23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="11"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E23" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="5">
         <v>12</v>
       </c>
@@ -2280,9 +2314,11 @@
       <c r="D24" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="11"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.05" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="8">
         <v>12</v>
       </c>
@@ -2295,7 +2331,93 @@
       <c r="D25" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="11"/>
+      <c r="E25" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A26" s="2">
+        <v>19</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A27" s="5">
+        <v>19</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A28" s="5">
+        <v>19</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A29" s="5">
+        <v>19</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A30" s="5">
+        <v>19</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.05" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="8">
+        <v>19</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E19"/>

</xml_diff>